<commit_message>
day 4 upto lcs
</commit_message>
<xml_diff>
--- a/takeuforward-dsa/takeuforward-dsa.xlsx
+++ b/takeuforward-dsa/takeuforward-dsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="175">
   <si>
     <t xml:space="preserve">Problem</t>
   </si>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">@ new row = top row[i]+ top row[i+1]</t>
   </si>
   <si>
-    <t xml:space="preserve">@ combination_result = comb_result+position/position-1</t>
+    <t xml:space="preserve">@ combination_result = comb_result+position/position+1</t>
   </si>
   <si>
     <t xml:space="preserve">@ given rowCposition rCp</t>
@@ -379,13 +379,202 @@
     <t xml:space="preserve">@ takes O(n) time complexity and O(1)space but it uses long long which is ambiguity</t>
   </si>
   <si>
-    <t xml:space="preserve">@ sum of nos = n(n+1)/2, sum of square = ((n+1)(2n+1))/2</t>
+    <t xml:space="preserve">@ sum of nos = n(n+1)/2, sum of square = (n(n+1)(2n+1))/6</t>
   </si>
   <si>
     <t xml:space="preserve">@ map with 0 is missing and with 2 is repeating number</t>
   </si>
   <si>
     <t xml:space="preserve">@ xor method is there but rare case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inversion of array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create 2 for loops and check for 2 nos which satisfy the condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use merge sort algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if it satisfies then add the count value by one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ we can create a count variable in return function </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n2) time complexity and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ whenever a swap occurs if right hand side has smaller value then set count as n_left – position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ in this way we can achieve count using O(n logn)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search in 2d matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ loop through entire array and search for the element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use binary search in this matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ you can change the binarysearch_index  by using divide and remainder of index with columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ row = index/nColumns, col = index%nColumns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power x, n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ calculate power by multiplying same number n times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use binary multiplication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if n is even then x=x*x, and n=n/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if n is odd then ans = ans*x and n=n-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">majority element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use hashmap on array element find the count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use moore voting algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ set count++ if element equals to arr element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use count to find maximum element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ set the count = 0 and element is first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now check whether the given number is maximum by iterating through arr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) time and space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if count is 0 then set element as arr element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ thus the maximum element is achieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">majority elements(more than one)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use hashmap on array element and find count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ count1 ++ if element equal to ele1 or count2++ if ele2 equals to arr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ count to find max element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create ele1 and ele2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ check whether the given nos are maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ count1 and count2 is zero </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ thus found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid unique paths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use recursion to find all possible solution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use recursion plus dp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ its a combination problem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n!) time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create arr and store all result in dp if same occurs then we can simply get from arr instead recursion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ we can simply find by m+n-2Cm-1 or m+n-2Cn-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(nxm) time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use for loop to find ncr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reverse pairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use 2 for loops to satisfy given condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use mergesort algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ when the array is splitted use the condition to calculate the count of array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(nlogn) time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use 2 for loops and find all possible sum value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a hashmap put condition first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if (arr[target-arrval]!=end)ans.push</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ put key as arr value and value as index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ dict[arr[i]]=i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">four sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use 3 for loops find all possiblities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use 2 pointer for loops and binary search last 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n3) time and O(1)space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n3) time and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use rem sum of 2 ptr value and compare rem by binary searching values</t>
   </si>
 </sst>
 </file>
@@ -543,7 +732,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -761,6 +950,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -841,18 +1038,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D76" activeCellId="0" sqref="D76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="61.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="83.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="83.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="121.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="2" width="9"/>
   </cols>
@@ -1365,8 +1562,300 @@
       </c>
       <c r="E44" s="21"/>
     </row>
+    <row r="45" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="40"/>
+    </row>
+    <row r="46" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="38"/>
+      <c r="C46" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="42"/>
+    </row>
+    <row r="47" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="38"/>
+      <c r="C47" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="42"/>
+    </row>
+    <row r="48" s="43" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="38"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="44"/>
+    </row>
+    <row r="49" s="45" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7"/>
+      <c r="C50" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E52" s="17"/>
+    </row>
+    <row r="53" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="15"/>
+      <c r="C53" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" s="50" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="55"/>
+    </row>
+    <row r="55" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="38"/>
+      <c r="C56" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" s="43" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="38"/>
+      <c r="C57" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" s="56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" s="45" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7"/>
+      <c r="C59" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7"/>
+      <c r="C60" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15"/>
+      <c r="C62" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" s="50" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="15"/>
+      <c r="C63" s="55"/>
+      <c r="D63" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="E63" s="55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" s="40"/>
+    </row>
+    <row r="65" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="38"/>
+      <c r="C65" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="E65" s="42"/>
+    </row>
+    <row r="66" s="43" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="38"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="E66" s="56"/>
+    </row>
+    <row r="67" s="45" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7"/>
+      <c r="C68" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E68" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" s="50" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15"/>
+      <c r="C70" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E70" s="21"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="26">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
@@ -1384,6 +1873,15 @@
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A70"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
day 6 one problem left
</commit_message>
<xml_diff>
--- a/takeuforward-dsa/takeuforward-dsa.xlsx
+++ b/takeuforward-dsa/takeuforward-dsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="196">
   <si>
     <t xml:space="preserve">Problem</t>
   </si>
@@ -620,6 +620,24 @@
   </si>
   <si>
     <t xml:space="preserve">@ takes O(n) space O(n)time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count no of subarr xor k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use 2 for loop to find all possible subarr and find xor val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use prefix xor and store the values and count of appearance as key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ the target subarr in arr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now if prefix xored to target gives me a value which is present in dict then it means there contains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ the count is used to get how many times it appeared</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1113,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C78" activeCellId="0" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1969,6 +1987,31 @@
       </c>
       <c r="E75" s="36" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recursion kinda tough ngl
</commit_message>
<xml_diff>
--- a/takeuforward-dsa/takeuforward-dsa.xlsx
+++ b/takeuforward-dsa/takeuforward-dsa.xlsx
@@ -1321,7 +1321,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1344,6 +1344,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBF819E"/>
         <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF10D0C"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -1415,7 +1421,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1568,27 +1574,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1613,7 +1623,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFF10D0C"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1679,8 +1689,8 @@
   </sheetPr>
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="A125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A131" activeCellId="0" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2064,7 +2074,7 @@
       </c>
     </row>
     <row r="33" s="33" customFormat="true" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="38" t="s">
         <v>82</v>
       </c>
       <c r="C33" s="34" t="s">
@@ -2076,7 +2086,7 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32"/>
+      <c r="A34" s="38"/>
       <c r="C34" s="36" t="s">
         <v>85</v>
       </c>
@@ -2086,7 +2096,7 @@
       <c r="E34" s="36"/>
     </row>
     <row r="35" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32"/>
+      <c r="A35" s="38"/>
       <c r="C35" s="36" t="s">
         <v>87</v>
       </c>
@@ -2096,7 +2106,7 @@
       <c r="E35" s="36"/>
     </row>
     <row r="36" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="32"/>
+      <c r="A36" s="38"/>
       <c r="C36" s="37" t="s">
         <v>89</v>
       </c>
@@ -2312,13 +2322,13 @@
     </row>
     <row r="57" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="32"/>
-      <c r="C57" s="38" t="s">
+      <c r="C57" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="D57" s="38" t="s">
+      <c r="D57" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="E57" s="38" t="s">
+      <c r="E57" s="39" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2419,11 +2429,11 @@
     </row>
     <row r="66" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="32"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38" t="s">
+      <c r="C66" s="39"/>
+      <c r="D66" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E66" s="38"/>
+      <c r="E66" s="39"/>
     </row>
     <row r="67" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
@@ -2560,7 +2570,7 @@
       </c>
     </row>
     <row r="78" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="38" t="s">
         <v>195</v>
       </c>
       <c r="C78" s="34" t="s">
@@ -2574,14 +2584,14 @@
       </c>
     </row>
     <row r="79" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="32"/>
-      <c r="C79" s="38" t="s">
+      <c r="A79" s="38"/>
+      <c r="C79" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="D79" s="38" t="s">
+      <c r="D79" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="E79" s="38"/>
+      <c r="E79" s="39"/>
     </row>
     <row r="80" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="7" t="s">
@@ -2643,11 +2653,11 @@
     </row>
     <row r="85" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="32"/>
-      <c r="C85" s="38" t="s">
+      <c r="C85" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
     </row>
     <row r="86" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="7" t="s">
@@ -2719,33 +2729,33 @@
     </row>
     <row r="92" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="32"/>
-      <c r="C92" s="38" t="s">
+      <c r="C92" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="E92" s="38"/>
-    </row>
-    <row r="93" s="40" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="39" t="s">
+      <c r="E92" s="39"/>
+    </row>
+    <row r="93" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="40" t="s">
         <v>234</v>
       </c>
-      <c r="C93" s="41" t="s">
+      <c r="C93" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="D93" s="41" t="s">
+      <c r="D93" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="E93" s="41"/>
-    </row>
-    <row r="94" s="42" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="39"/>
-      <c r="C94" s="43" t="s">
+      <c r="E93" s="42"/>
+    </row>
+    <row r="94" s="43" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="40"/>
+      <c r="C94" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="D94" s="43"/>
-      <c r="E94" s="43"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
     </row>
     <row r="95" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="14" t="s">
@@ -2783,13 +2793,13 @@
     </row>
     <row r="98" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="32"/>
-      <c r="C98" s="38" t="s">
+      <c r="C98" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="D98" s="38" t="s">
+      <c r="D98" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="E98" s="38"/>
+      <c r="E98" s="39"/>
     </row>
     <row r="99" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="7" t="s">
@@ -2863,13 +2873,13 @@
     </row>
     <row r="105" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="32"/>
-      <c r="C105" s="38" t="s">
+      <c r="C105" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="D105" s="38" t="s">
+      <c r="D105" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="E105" s="38"/>
+      <c r="E105" s="39"/>
     </row>
     <row r="106" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="7" t="s">
@@ -2937,13 +2947,13 @@
     </row>
     <row r="111" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="32"/>
-      <c r="C111" s="38" t="s">
+      <c r="C111" s="39" t="s">
         <v>282</v>
       </c>
-      <c r="D111" s="38" t="s">
+      <c r="D111" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="E111" s="38" t="s">
+      <c r="E111" s="39" t="s">
         <v>284</v>
       </c>
     </row>
@@ -2972,7 +2982,7 @@
       <c r="E113" s="29"/>
     </row>
     <row r="114" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="14" t="s">
+      <c r="A114" s="38" t="s">
         <v>291</v>
       </c>
       <c r="C114" s="16" t="s">
@@ -2986,7 +2996,7 @@
       </c>
     </row>
     <row r="115" s="19" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="14"/>
+      <c r="A115" s="38"/>
       <c r="C115" s="18" t="s">
         <v>295</v>
       </c>
@@ -2996,7 +3006,7 @@
       <c r="E115" s="18"/>
     </row>
     <row r="116" s="21" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="14"/>
+      <c r="A116" s="38"/>
       <c r="C116" s="20" t="s">
         <v>297</v>
       </c>
@@ -3019,13 +3029,13 @@
     </row>
     <row r="118" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="32"/>
-      <c r="C118" s="38" t="s">
+      <c r="C118" s="39" t="s">
         <v>302</v>
       </c>
-      <c r="D118" s="38" t="s">
+      <c r="D118" s="39" t="s">
         <v>303</v>
       </c>
-      <c r="E118" s="38"/>
+      <c r="E118" s="39"/>
     </row>
     <row r="119" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="7" t="s">
@@ -3076,7 +3086,7 @@
       </c>
     </row>
     <row r="123" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="44" t="s">
+      <c r="A123" s="45" t="s">
         <v>315</v>
       </c>
       <c r="C123" s="36" t="s">
@@ -3090,7 +3100,7 @@
       </c>
     </row>
     <row r="124" s="35" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="44"/>
+      <c r="A124" s="45"/>
       <c r="C124" s="36" t="s">
         <v>319</v>
       </c>
@@ -3123,7 +3133,7 @@
       </c>
     </row>
     <row r="127" s="19" customFormat="true" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="45" t="s">
+      <c r="A127" s="46" t="s">
         <v>327</v>
       </c>
       <c r="C127" s="19" t="s">
@@ -3137,7 +3147,7 @@
       </c>
     </row>
     <row r="128" s="19" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="45"/>
+      <c r="A128" s="46"/>
       <c r="C128" s="19" t="s">
         <v>330</v>
       </c>
@@ -3146,7 +3156,7 @@
       </c>
     </row>
     <row r="129" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="44" t="s">
+      <c r="A129" s="45" t="s">
         <v>332</v>
       </c>
       <c r="C129" s="35" t="s">
@@ -3157,7 +3167,7 @@
       </c>
     </row>
     <row r="130" s="35" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="44"/>
+      <c r="A130" s="45"/>
       <c r="C130" s="35" t="s">
         <v>335</v>
       </c>

</xml_diff>

<commit_message>
binary search going on
</commit_message>
<xml_diff>
--- a/takeuforward-dsa/takeuforward-dsa.xlsx
+++ b/takeuforward-dsa/takeuforward-dsa.xlsx
@@ -1850,8 +1850,8 @@
   </sheetPr>
   <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A179" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3143,7 +3143,7 @@
       <c r="E113" s="29"/>
     </row>
     <row r="114" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="14" t="s">
         <v>291</v>
       </c>
       <c r="C114" s="16" t="s">
@@ -3157,7 +3157,7 @@
       </c>
     </row>
     <row r="115" s="19" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="39"/>
+      <c r="A115" s="14"/>
       <c r="C115" s="18" t="s">
         <v>295</v>
       </c>
@@ -3167,7 +3167,7 @@
       <c r="E115" s="18"/>
     </row>
     <row r="116" s="21" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="39"/>
+      <c r="A116" s="14"/>
       <c r="C116" s="20" t="s">
         <v>297</v>
       </c>

</xml_diff>

<commit_message>
binary trees on progress
</commit_message>
<xml_diff>
--- a/takeuforward-dsa/takeuforward-dsa.xlsx
+++ b/takeuforward-dsa/takeuforward-dsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="609">
   <si>
     <t xml:space="preserve">Problem</t>
   </si>
@@ -1718,6 +1718,543 @@
   </si>
   <si>
     <t xml:space="preserve">@ pop the maxheap untill k and return the top pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement stack using arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a array and push the values to the end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ for removal set the topmost value to -1 and reduce ptr and size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ maintain size and a pointer to note down the last position of add/removal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) space and O(1)time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if user asks specific method add the pointer and size to add the value inside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement queue using arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a array and 2 ptr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ for removal make ptr1 value as -1 and add ptr1 by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ user ptr1 as start node and ptr2 as end node as for a queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ there will be an edge case where ptr1 gets till size and ptr2 is at max size in these cases we can tackle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ when a user add a value increase ptr 2 and set value for it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ by using modulo of the given capacity of the queue such that ptr1-ptr2 == size. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement stack using queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ insert the value in the queue at back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) for every removal 2 times to rotate and rerotate the queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ during removal rotate the entire queue by size-1 times and then return the value which is LIFO in nature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement queue using stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ during insert push the values in stack 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(2n) time and O(2n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ when on removal push every element from stack1 to stack 2 unitll it is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ when it is empty remove stack 2 top which is the first inserted value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balanced paranthesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a stack to store the open bracket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if stack is empty then it is balanced or else unbalanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if close bracket occurs then pop the open bracket and go to nxt value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if stack is empty before end bracket then return unbalanced/false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ then continue till the end of string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">next greater element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ using a monotonically greater stack from behind 2n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) time an dO(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ we can find the greater element from behind to start such that we find the element very greater from the index </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort a stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ we can sort a stack using recursion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ push the value in the stack as ordered way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a top element n and go on recursion untill stack is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ check whether the top value is less than the nth value of inserting stack if yes then push it or else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create recursion on this stack untill the top value is set to its correct position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">next smaller element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a stack and start iteration from 0 to end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now it will form next smaller element based on the current index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now store the elements in the stack as per small order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if cur element is greater than stack then remove all element greater than start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRU Cache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ lru cache is a important problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ since it is the condition of the cache to be remembered for calling it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ we have to create a hashmap and a doubly linked list fot this </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ it takes O(1) time and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ in get method if map doesnt contain value return -1 or return the map value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ similarly for insert create a new node and store in the head. If overflow then remove the tail value LRU i mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ but for every calling of get method you have to send the node to the start </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largest rectangle in histogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a stack to store the next smaller value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ thus we return the diff multiplied by len to give max area of rectangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ after going through entire array from reverse find the smaller value in both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(3n) time and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ the difference b/w both direction is the rectangle size of that particular len</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sliding window maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a queue to store the value if the ptr contain size of window-1 then </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) time and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ subtract and remove the last value by popping the first. A deque will be useful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement min stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@  use sort stack in the insertion of the values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ everything similar to stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotten oranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use a queue to store the next values and run loop untill empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now the queue is pushed and rotten one is deleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ add timer when fresh oranges are present near rotten ones after every addn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ run this same  loop untill queue becomes empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ return the max time among the finding calculation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock span problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a pair of stack and store the values and count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ return the addn of every stock span</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if top value of stack is less than the stack new value add it to the new pair +1 and go on the path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find maximum and minimum of every window size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use queue and stack problem in this question sliding window and for loops for every window size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n*n) time and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celebrity problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a stack and store every index of the array find whether top and top-1 values [0][1] and [1][0] contain 1 if it contains then add that into stack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(m+n) time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ continue this untill you find a celebrity who has 0 in everything </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reverse words in string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create 2 ptr values start and end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now push the substring to a string ans and append the substring like ans = substr+ans</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">@ move start clear out the spaces before start of the 1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> word</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">@ thus we can reverse the entire string and get the answer </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">@ then set 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ptr at that letter and go untill a space is occured</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">longest palindrome in string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ go through entire array and select a particular string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ run 2 while loops as even and odd calcuate the max palindrome value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ then return the max which is the answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roman to integer and viceversa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ to calculate roman to int we create hashmap for roman literals and go through array from start </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n) and O(1) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ when the s[i+1] is greater than s[i] then minus that particular value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement atoi/strstr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ remove spaces before start of the string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ thus we arrive at the current value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ check if only string in between 0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ to avoid overflow of number INTMAX we divide intmax/10 and check whether cur is greater than intmax return it or else if nxt number is close to remainder of intmax return it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ then we can find the number by calculation *10+cur value-’0’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ check for the symbol before the value too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longest common prefix</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">@ set 2 ptr from 0</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> arr and 1-nth aray</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create common prefix by checking untill where it is same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ use a for loop from 1 to n and check for same prefixes using 2 ptr approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ finally u will arrive at a value where both will be same </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ return it that will be the answer(takes O(n) time and O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check for anagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a 256 size array for every character in the string with boolean values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now in the second string continue till the end of the array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(256*3) time and space</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">@ go through 1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> array and add 1 to it</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now u have to subtract the values.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">@ after going through every array adding  1 to found characters get to 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> string</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">@ run another loop to find the arr has 0 in it if it is continued to be 0 return true orelse return false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count and say</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ from string starting from 3 to n set start as 11 and add $ to the end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n*m) time ans O(n) space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ now start counting . If the cur string is not equal to str-1 then add it to new tmp then add count and value as string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ thus after each iteration move new tmp as ans </t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare version number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ create a integer n and m for both version of string to be compared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ if at all anything greater and less than return the value accordingly or else continue to nxt value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ continue untill the string comes to end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ find the number before each dot in the string then compare both numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ 0 before the number  values nothing in here </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ return the values accordingly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ takes O(n*m) time and space</t>
   </si>
 </sst>
 </file>
@@ -2158,10 +2695,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F185"/>
+  <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A170" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A187" activeCellId="0" sqref="A187"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A230" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A251" activeCellId="0" sqref="A251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4237,8 +4774,581 @@
         <v>479</v>
       </c>
     </row>
+    <row r="186" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A186" s="45" t="s">
+        <v>480</v>
+      </c>
+      <c r="C186" s="46" t="s">
+        <v>481</v>
+      </c>
+      <c r="D186" s="46" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="187" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="45"/>
+      <c r="C187" s="47" t="s">
+        <v>483</v>
+      </c>
+      <c r="D187" s="47" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="188" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="45"/>
+      <c r="C188" s="48" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="189" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A189" s="32" t="s">
+        <v>486</v>
+      </c>
+      <c r="C189" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="D189" s="33" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="190" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="32"/>
+      <c r="C190" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="D190" s="35" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="191" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="32"/>
+      <c r="C191" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="D191" s="37" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="192" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A192" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="D192" s="10" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="193" s="13" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="7"/>
+      <c r="C193" s="13" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="194" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A194" s="45" t="s">
+        <v>497</v>
+      </c>
+      <c r="C194" s="46" t="s">
+        <v>498</v>
+      </c>
+      <c r="D194" s="46" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="195" s="47" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="45"/>
+      <c r="C195" s="47" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="196" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="45"/>
+      <c r="C196" s="48" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="197" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A197" s="32" t="s">
+        <v>502</v>
+      </c>
+      <c r="C197" s="33" t="s">
+        <v>503</v>
+      </c>
+      <c r="D197" s="33" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="198" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="32"/>
+      <c r="C198" s="35" t="s">
+        <v>505</v>
+      </c>
+      <c r="D198" s="35" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="199" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="32"/>
+      <c r="C199" s="37" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="200" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A200" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="D200" s="10" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="201" s="13" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="7"/>
+      <c r="C201" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="202" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A202" s="45" t="s">
+        <v>512</v>
+      </c>
+      <c r="C202" s="46" t="s">
+        <v>513</v>
+      </c>
+      <c r="D202" s="46" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="203" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="45"/>
+      <c r="C203" s="47" t="s">
+        <v>515</v>
+      </c>
+      <c r="D203" s="47" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="204" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="45"/>
+      <c r="D204" s="48" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="205" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A205" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="C205" s="33" t="s">
+        <v>519</v>
+      </c>
+      <c r="D205" s="33" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="206" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="32"/>
+      <c r="C206" s="35" t="s">
+        <v>521</v>
+      </c>
+      <c r="D206" s="35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="207" s="37" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="32"/>
+      <c r="C207" s="37" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="208" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A208" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="C208" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="D208" s="10" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="209" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="7"/>
+      <c r="C209" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="D209" s="12" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="210" s="12" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="7"/>
+      <c r="C210" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="D210" s="12" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="211" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="7"/>
+      <c r="C211" s="13" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="212" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A212" s="45" t="s">
+        <v>531</v>
+      </c>
+      <c r="C212" s="46" t="s">
+        <v>532</v>
+      </c>
+      <c r="D212" s="46" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="213" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="45"/>
+      <c r="C213" s="47" t="s">
+        <v>534</v>
+      </c>
+      <c r="D213" s="47" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="214" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="45"/>
+      <c r="C214" s="48" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="215" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A215" s="32" t="s">
+        <v>537</v>
+      </c>
+      <c r="C215" s="33" t="s">
+        <v>538</v>
+      </c>
+      <c r="D215" s="33" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="216" s="37" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="32"/>
+      <c r="C216" s="37" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="217" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A217" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="C217" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="D217" s="10" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="218" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="7"/>
+      <c r="C218" s="13" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="219" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A219" s="45" t="s">
+        <v>544</v>
+      </c>
+      <c r="C219" s="46" t="s">
+        <v>545</v>
+      </c>
+      <c r="D219" s="46" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="220" s="47" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="45"/>
+      <c r="C220" s="47" t="s">
+        <v>547</v>
+      </c>
+      <c r="D220" s="47" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="221" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="45"/>
+      <c r="D221" s="48" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="222" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A222" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="C222" s="33" t="s">
+        <v>551</v>
+      </c>
+      <c r="D222" s="33" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="223" s="37" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="32"/>
+      <c r="C223" s="37" t="s">
+        <v>553</v>
+      </c>
+      <c r="D223" s="37" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="224" s="10" customFormat="true" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A224" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="C224" s="10" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="225" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="7"/>
+      <c r="C225" s="13" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="226" s="46" customFormat="true" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A226" s="45" t="s">
+        <v>557</v>
+      </c>
+      <c r="C226" s="46" t="s">
+        <v>558</v>
+      </c>
+      <c r="D226" s="46" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="227" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="45"/>
+      <c r="C227" s="48" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="228" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A228" s="32" t="s">
+        <v>561</v>
+      </c>
+      <c r="C228" s="33" t="s">
+        <v>562</v>
+      </c>
+      <c r="D228" s="33" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="229" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="32"/>
+      <c r="C229" s="35" t="s">
+        <v>564</v>
+      </c>
+      <c r="D229" s="35" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="230" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="32"/>
+      <c r="C230" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="D230" s="37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="231" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A231" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="C231" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="D231" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="232" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="7"/>
+      <c r="C232" s="12" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="233" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="7"/>
+      <c r="C233" s="13" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="234" s="46" customFormat="true" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A234" s="45" t="s">
+        <v>571</v>
+      </c>
+      <c r="C234" s="46" t="s">
+        <v>572</v>
+      </c>
+      <c r="D234" s="46" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="235" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="45"/>
+      <c r="C235" s="48" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="236" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A236" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="C236" s="33" t="s">
+        <v>576</v>
+      </c>
+      <c r="D236" s="33" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="237" s="35" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="32"/>
+      <c r="C237" s="35" t="s">
+        <v>578</v>
+      </c>
+      <c r="D237" s="35" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="238" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="32"/>
+      <c r="C238" s="37" t="s">
+        <v>580</v>
+      </c>
+      <c r="D238" s="37" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="239" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A239" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="C239" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="D239" s="10" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="240" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="7"/>
+      <c r="C240" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="D240" s="12" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="241" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="7"/>
+      <c r="D241" s="13" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="242" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A242" s="45" t="s">
+        <v>588</v>
+      </c>
+      <c r="C242" s="46" t="s">
+        <v>589</v>
+      </c>
+      <c r="D242" s="46" t="s">
+        <v>590</v>
+      </c>
+      <c r="E242" s="46" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="243" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="45"/>
+      <c r="C243" s="47" t="s">
+        <v>592</v>
+      </c>
+      <c r="D243" s="47" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="244" s="48" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="45"/>
+      <c r="C244" s="48" t="s">
+        <v>594</v>
+      </c>
+      <c r="D244" s="48" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="245" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A245" s="32" t="s">
+        <v>596</v>
+      </c>
+      <c r="C245" s="33" t="s">
+        <v>597</v>
+      </c>
+      <c r="D245" s="33" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="246" s="35" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="32"/>
+      <c r="C246" s="35" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="247" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="32"/>
+      <c r="C247" s="37" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="248" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A248" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="C248" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="D248" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="E248" s="10" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="249" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="7"/>
+      <c r="C249" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="D249" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="E249" s="12" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="250" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="7"/>
+      <c r="E250" s="13" t="s">
+        <v>608</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="103">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
@@ -4318,6 +5428,30 @@
     <mergeCell ref="A177:A179"/>
     <mergeCell ref="A180:A182"/>
     <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="A189:A191"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A194:A196"/>
+    <mergeCell ref="A197:A199"/>
+    <mergeCell ref="A200:A201"/>
+    <mergeCell ref="A202:A204"/>
+    <mergeCell ref="A205:A207"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="A212:A214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="A219:A221"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="A224:A225"/>
+    <mergeCell ref="A226:A227"/>
+    <mergeCell ref="A228:A230"/>
+    <mergeCell ref="A231:A233"/>
+    <mergeCell ref="A234:A235"/>
+    <mergeCell ref="A236:A238"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="A245:A247"/>
+    <mergeCell ref="A248:A250"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>